<commit_message>
Analizador Semántico en funcionamiento
</commit_message>
<xml_diff>
--- a/TablaSintactica.xlsx
+++ b/TablaSintactica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\OneDrive\Documentos\University\Archivos\PDF's\Autómatas\Programas\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E1B00-B237-4E5F-B86A-F160B67499F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2E49C-89ED-4ED1-A9BB-4FC8C01D7A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{D62EC496-1556-4E0C-9A3E-7AF50D9FA4F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{D62EC496-1556-4E0C-9A3E-7AF50D9FA4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -831,12 +831,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -851,7 +857,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -878,6 +884,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1196,18 +1208,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E59CA23-57F3-4C77-80B4-8B27E4C8042E}">
   <dimension ref="A1:CY164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="44" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="45" max="45" width="12.33203125" customWidth="1"/>
-    <col min="46" max="46" width="12.6640625" customWidth="1"/>
-    <col min="47" max="47" width="14.19921875" customWidth="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1"/>
+    <col min="46" max="46" width="12.7109375" customWidth="1"/>
+    <col min="47" max="47" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
@@ -1637,7 +1649,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>101</v>
       </c>
@@ -1703,7 +1715,7 @@
       <c r="BE3" s="2"/>
       <c r="BF3" s="2"/>
     </row>
-    <row r="4" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1767,7 +1779,7 @@
       <c r="BE4" s="3"/>
       <c r="BF4" s="3"/>
     </row>
-    <row r="5" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1831,7 +1843,7 @@
       <c r="BE5" s="3"/>
       <c r="BF5" s="3"/>
     </row>
-    <row r="6" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1895,7 +1907,7 @@
       <c r="BE6" s="3"/>
       <c r="BF6" s="3"/>
     </row>
-    <row r="7" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1959,7 +1971,7 @@
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>
     </row>
-    <row r="8" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2051,7 +2063,7 @@
       <c r="BE8" s="3"/>
       <c r="BF8" s="3"/>
     </row>
-    <row r="9" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2115,7 +2127,7 @@
       <c r="BE9" s="3"/>
       <c r="BF9" s="3"/>
     </row>
-    <row r="10" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2189,7 +2201,7 @@
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
     </row>
-    <row r="11" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2253,7 +2265,7 @@
       <c r="BE11" s="3"/>
       <c r="BF11" s="3"/>
     </row>
-    <row r="12" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2317,7 +2329,7 @@
       <c r="BE12" s="3"/>
       <c r="BF12" s="3"/>
     </row>
-    <row r="13" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2381,7 +2393,7 @@
       <c r="BE13" s="3"/>
       <c r="BF13" s="3"/>
     </row>
-    <row r="14" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -2445,7 +2457,7 @@
       <c r="BE14" s="3"/>
       <c r="BF14" s="3"/>
     </row>
-    <row r="15" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2509,7 +2521,7 @@
       <c r="BE15" s="3"/>
       <c r="BF15" s="3"/>
     </row>
-    <row r="16" spans="1:62" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2573,7 +2585,7 @@
       <c r="BE16" s="3"/>
       <c r="BF16" s="3"/>
     </row>
-    <row r="17" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2639,7 +2651,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2713,7 +2725,7 @@
       <c r="BE18" s="3"/>
       <c r="BF18" s="3"/>
     </row>
-    <row r="19" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2777,7 +2789,7 @@
       <c r="BE19" s="3"/>
       <c r="BF19" s="3"/>
     </row>
-    <row r="20" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -2841,7 +2853,7 @@
       <c r="BE20" s="3"/>
       <c r="BF20" s="3"/>
     </row>
-    <row r="21" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2905,7 +2917,7 @@
       <c r="BE21" s="3"/>
       <c r="BF21" s="3"/>
     </row>
-    <row r="22" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -2977,7 +2989,7 @@
       <c r="BE22" s="3"/>
       <c r="BF22" s="3"/>
     </row>
-    <row r="23" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3041,7 +3053,7 @@
       <c r="BE23" s="3"/>
       <c r="BF23" s="3"/>
     </row>
-    <row r="24" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3105,7 +3117,7 @@
       <c r="BE24" s="3"/>
       <c r="BF24" s="3"/>
     </row>
-    <row r="25" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3169,7 +3181,7 @@
       <c r="BE25" s="3"/>
       <c r="BF25" s="3"/>
     </row>
-    <row r="26" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3233,7 +3245,7 @@
       <c r="BE26" s="3"/>
       <c r="BF26" s="3"/>
     </row>
-    <row r="27" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3311,7 +3323,7 @@
       <c r="BE27" s="3"/>
       <c r="BF27" s="3"/>
     </row>
-    <row r="28" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -3389,7 +3401,7 @@
       <c r="BE28" s="3"/>
       <c r="BF28" s="3"/>
     </row>
-    <row r="29" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -3459,7 +3471,7 @@
       <c r="BE29" s="3"/>
       <c r="BF29" s="3"/>
     </row>
-    <row r="30" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -3523,7 +3535,7 @@
       <c r="BE30" s="3"/>
       <c r="BF30" s="3"/>
     </row>
-    <row r="31" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -3613,7 +3625,7 @@
       <c r="BE31" s="3"/>
       <c r="BF31" s="3"/>
     </row>
-    <row r="32" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -3677,7 +3689,7 @@
       <c r="BE32" s="3"/>
       <c r="BF32" s="3"/>
     </row>
-    <row r="33" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -3741,7 +3753,7 @@
       <c r="BE33" s="3"/>
       <c r="BF33" s="3"/>
     </row>
-    <row r="34" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -3809,7 +3821,7 @@
       <c r="BE34" s="3"/>
       <c r="BF34" s="3"/>
     </row>
-    <row r="35" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
@@ -3875,7 +3887,7 @@
       <c r="BE35" s="3"/>
       <c r="BF35" s="3"/>
     </row>
-    <row r="36" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -3941,7 +3953,7 @@
       <c r="BE36" s="3"/>
       <c r="BF36" s="3"/>
     </row>
-    <row r="37" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
@@ -4007,7 +4019,7 @@
       <c r="BE37" s="3"/>
       <c r="BF37" s="3"/>
     </row>
-    <row r="38" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -4079,7 +4091,7 @@
       <c r="BE38" s="3"/>
       <c r="BF38" s="3"/>
     </row>
-    <row r="39" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
@@ -4157,7 +4169,7 @@
       <c r="BE39" s="3"/>
       <c r="BF39" s="3"/>
     </row>
-    <row r="40" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
@@ -4221,7 +4233,7 @@
       <c r="BE40" s="3"/>
       <c r="BF40" s="3"/>
     </row>
-    <row r="41" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
@@ -4247,8 +4259,8 @@
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
-      <c r="X41" s="3" t="s">
-        <v>40</v>
+      <c r="X41" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
@@ -4285,7 +4297,7 @@
       <c r="BE41" s="3"/>
       <c r="BF41" s="3"/>
     </row>
-    <row r="42" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -4363,7 +4375,7 @@
       <c r="BE42" s="3"/>
       <c r="BF42" s="3"/>
     </row>
-    <row r="43" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -4441,7 +4453,7 @@
       <c r="BE43" s="3"/>
       <c r="BF43" s="3"/>
     </row>
-    <row r="44" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>40</v>
       </c>
@@ -4505,7 +4517,7 @@
       <c r="BE44" s="3"/>
       <c r="BF44" s="3"/>
     </row>
-    <row r="45" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>41</v>
       </c>
@@ -4569,7 +4581,7 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
@@ -4661,7 +4673,7 @@
       <c r="BE46" s="3"/>
       <c r="BF46" s="3"/>
     </row>
-    <row r="47" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -4753,7 +4765,7 @@
       <c r="BE47" s="3"/>
       <c r="BF47" s="3"/>
     </row>
-    <row r="48" spans="1:58" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
@@ -4817,7 +4829,7 @@
       <c r="BE48" s="3"/>
       <c r="BF48" s="3"/>
     </row>
-    <row r="49" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>45</v>
       </c>
@@ -4938,7 +4950,7 @@
       <c r="CX49" s="4"/>
       <c r="CY49" s="4"/>
     </row>
-    <row r="50" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -5047,7 +5059,7 @@
       <c r="CX50" s="4"/>
       <c r="CY50" s="4"/>
     </row>
-    <row r="51" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>105</v>
       </c>
@@ -5156,7 +5168,7 @@
       <c r="CX51" s="4"/>
       <c r="CY51" s="4"/>
     </row>
-    <row r="52" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>106</v>
       </c>
@@ -5265,7 +5277,7 @@
       <c r="CX52" s="4"/>
       <c r="CY52" s="4"/>
     </row>
-    <row r="53" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>107</v>
       </c>
@@ -5380,7 +5392,7 @@
       <c r="CX53" s="4"/>
       <c r="CY53" s="4"/>
     </row>
-    <row r="54" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>108</v>
       </c>
@@ -5489,7 +5501,7 @@
       <c r="CX54" s="4"/>
       <c r="CY54" s="4"/>
     </row>
-    <row r="55" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>109</v>
       </c>
@@ -5598,7 +5610,7 @@
       <c r="CX55" s="4"/>
       <c r="CY55" s="4"/>
     </row>
-    <row r="56" spans="1:103" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -5707,7 +5719,7 @@
       <c r="CX56" s="4"/>
       <c r="CY56" s="4"/>
     </row>
-    <row r="57" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>111</v>
       </c>
@@ -5816,7 +5828,7 @@
       <c r="CX57" s="4"/>
       <c r="CY57" s="4"/>
     </row>
-    <row r="58" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
@@ -5929,7 +5941,7 @@
       <c r="CX58" s="4"/>
       <c r="CY58" s="4"/>
     </row>
-    <row r="59" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>113</v>
       </c>
@@ -6050,7 +6062,7 @@
       <c r="CX59" s="4"/>
       <c r="CY59" s="4"/>
     </row>
-    <row r="60" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>141</v>
       </c>
@@ -6167,7 +6179,7 @@
       <c r="CX60" s="4"/>
       <c r="CY60" s="4"/>
     </row>
-    <row r="61" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>142</v>
       </c>
@@ -6276,7 +6288,7 @@
       <c r="CX61" s="4"/>
       <c r="CY61" s="4"/>
     </row>
-    <row r="62" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -6409,7 +6421,7 @@
       <c r="CX62" s="4"/>
       <c r="CY62" s="4"/>
     </row>
-    <row r="63" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>144</v>
       </c>
@@ -6530,7 +6542,7 @@
       <c r="CX63" s="4"/>
       <c r="CY63" s="4"/>
     </row>
-    <row r="64" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>145</v>
       </c>
@@ -6645,7 +6657,7 @@
       <c r="CX64" s="4"/>
       <c r="CY64" s="4"/>
     </row>
-    <row r="65" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>146</v>
       </c>
@@ -6764,7 +6776,7 @@
       <c r="CX65" s="4"/>
       <c r="CY65" s="4"/>
     </row>
-    <row r="66" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>147</v>
       </c>
@@ -6883,7 +6895,7 @@
       <c r="CX66" s="4"/>
       <c r="CY66" s="4"/>
     </row>
-    <row r="67" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>149</v>
       </c>
@@ -6992,7 +7004,7 @@
       <c r="CX67" s="4"/>
       <c r="CY67" s="4"/>
     </row>
-    <row r="68" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>150</v>
       </c>
@@ -7101,7 +7113,7 @@
       <c r="CX68" s="4"/>
       <c r="CY68" s="4"/>
     </row>
-    <row r="69" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>151</v>
       </c>
@@ -7210,7 +7222,7 @@
       <c r="CX69" s="4"/>
       <c r="CY69" s="4"/>
     </row>
-    <row r="70" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>152</v>
       </c>
@@ -7319,7 +7331,7 @@
       <c r="CX70" s="4"/>
       <c r="CY70" s="4"/>
     </row>
-    <row r="71" spans="1:103" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>153</v>
       </c>
@@ -7428,7 +7440,7 @@
       <c r="CX71" s="4"/>
       <c r="CY71" s="4"/>
     </row>
-    <row r="72" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>154</v>
       </c>
@@ -7527,7 +7539,7 @@
       <c r="BZ72" s="9"/>
       <c r="CA72" s="9"/>
     </row>
-    <row r="73" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>155</v>
       </c>
@@ -7626,7 +7638,7 @@
       <c r="BZ73" s="9"/>
       <c r="CA73" s="9"/>
     </row>
-    <row r="74" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>157</v>
       </c>
@@ -7715,7 +7727,7 @@
       <c r="BZ74" s="9"/>
       <c r="CA74" s="9"/>
     </row>
-    <row r="75" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>158</v>
       </c>
@@ -7810,7 +7822,7 @@
       <c r="BZ75" s="9"/>
       <c r="CA75" s="9"/>
     </row>
-    <row r="76" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>159</v>
       </c>
@@ -7905,7 +7917,7 @@
       <c r="BZ76" s="9"/>
       <c r="CA76" s="9"/>
     </row>
-    <row r="77" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>160</v>
       </c>
@@ -8000,7 +8012,7 @@
       <c r="BZ77" s="9"/>
       <c r="CA77" s="9"/>
     </row>
-    <row r="78" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>161</v>
       </c>
@@ -8095,7 +8107,7 @@
       <c r="BZ78" s="9"/>
       <c r="CA78" s="9"/>
     </row>
-    <row r="79" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>162</v>
       </c>
@@ -8190,7 +8202,7 @@
       <c r="BZ79" s="9"/>
       <c r="CA79" s="9"/>
     </row>
-    <row r="80" spans="1:103" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:103" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>163</v>
       </c>
@@ -8285,7 +8297,7 @@
       <c r="BZ80" s="9"/>
       <c r="CA80" s="9"/>
     </row>
-    <row r="81" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>164</v>
       </c>
@@ -8384,7 +8396,7 @@
       <c r="BZ81" s="9"/>
       <c r="CA81" s="9"/>
     </row>
-    <row r="82" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>165</v>
       </c>
@@ -8469,7 +8481,7 @@
       <c r="BZ82" s="9"/>
       <c r="CA82" s="9"/>
     </row>
-    <row r="83" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>168</v>
       </c>
@@ -8554,7 +8566,7 @@
       <c r="BZ83" s="9"/>
       <c r="CA83" s="9"/>
     </row>
-    <row r="84" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>166</v>
       </c>
@@ -8643,7 +8655,7 @@
       <c r="BZ84" s="9"/>
       <c r="CA84" s="9"/>
     </row>
-    <row r="85" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>167</v>
       </c>
@@ -8732,7 +8744,7 @@
       <c r="BZ85" s="9"/>
       <c r="CA85" s="9"/>
     </row>
-    <row r="86" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>176</v>
       </c>
@@ -8817,7 +8829,7 @@
       <c r="BZ86" s="9"/>
       <c r="CA86" s="9"/>
     </row>
-    <row r="87" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>175</v>
       </c>
@@ -8914,7 +8926,7 @@
       <c r="BZ87" s="9"/>
       <c r="CA87" s="9"/>
     </row>
-    <row r="88" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>170</v>
       </c>
@@ -9011,7 +9023,7 @@
       <c r="BZ88" s="9"/>
       <c r="CA88" s="9"/>
     </row>
-    <row r="89" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>171</v>
       </c>
@@ -9108,7 +9120,7 @@
       <c r="BZ89" s="9"/>
       <c r="CA89" s="9"/>
     </row>
-    <row r="90" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>172</v>
       </c>
@@ -9205,7 +9217,7 @@
       <c r="BZ90" s="9"/>
       <c r="CA90" s="9"/>
     </row>
-    <row r="91" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>173</v>
       </c>
@@ -9302,7 +9314,7 @@
       <c r="BZ91" s="9"/>
       <c r="CA91" s="9"/>
     </row>
-    <row r="92" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>174</v>
       </c>
@@ -9387,7 +9399,7 @@
       <c r="BZ92" s="9"/>
       <c r="CA92" s="9"/>
     </row>
-    <row r="93" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>177</v>
       </c>
@@ -9480,7 +9492,7 @@
       <c r="BZ93" s="9"/>
       <c r="CA93" s="9"/>
     </row>
-    <row r="94" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>178</v>
       </c>
@@ -9573,7 +9585,7 @@
       <c r="BZ94" s="9"/>
       <c r="CA94" s="9"/>
     </row>
-    <row r="95" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>179</v>
       </c>
@@ -9658,7 +9670,7 @@
       <c r="BZ95" s="9"/>
       <c r="CA95" s="9"/>
     </row>
-    <row r="96" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>180</v>
       </c>
@@ -9747,7 +9759,7 @@
       <c r="BZ96" s="9"/>
       <c r="CA96" s="9"/>
     </row>
-    <row r="97" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>181</v>
       </c>
@@ -9836,7 +9848,7 @@
       <c r="BZ97" s="9"/>
       <c r="CA97" s="9"/>
     </row>
-    <row r="98" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>182</v>
       </c>
@@ -9933,7 +9945,7 @@
       <c r="BZ98" s="9"/>
       <c r="CA98" s="9"/>
     </row>
-    <row r="99" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>183</v>
       </c>
@@ -10030,7 +10042,7 @@
       <c r="BZ99" s="9"/>
       <c r="CA99" s="9"/>
     </row>
-    <row r="100" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>184</v>
       </c>
@@ -10125,7 +10137,7 @@
       <c r="BZ100" s="10"/>
       <c r="CA100" s="10"/>
     </row>
-    <row r="101" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>188</v>
       </c>
@@ -10220,7 +10232,7 @@
       <c r="BZ101" s="10"/>
       <c r="CA101" s="10"/>
     </row>
-    <row r="102" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>196</v>
       </c>
@@ -10309,7 +10321,7 @@
       <c r="BZ102" s="10"/>
       <c r="CA102" s="10"/>
     </row>
-    <row r="103" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>197</v>
       </c>
@@ -10406,7 +10418,7 @@
       <c r="BZ103" s="10"/>
       <c r="CA103" s="10"/>
     </row>
-    <row r="104" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>198</v>
       </c>
@@ -10491,7 +10503,7 @@
       <c r="BZ104" s="10"/>
       <c r="CA104" s="10"/>
     </row>
-    <row r="105" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>200</v>
       </c>
@@ -10576,7 +10588,7 @@
       <c r="BZ105" s="10"/>
       <c r="CA105" s="10"/>
     </row>
-    <row r="106" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>199</v>
       </c>
@@ -10667,7 +10679,7 @@
       <c r="BZ106" s="10"/>
       <c r="CA106" s="10"/>
     </row>
-    <row r="107" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>202</v>
       </c>
@@ -10752,7 +10764,7 @@
       <c r="BZ107" s="9"/>
       <c r="CA107" s="9"/>
     </row>
-    <row r="108" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>203</v>
       </c>
@@ -10837,7 +10849,7 @@
       <c r="BZ108" s="10"/>
       <c r="CA108" s="10"/>
     </row>
-    <row r="109" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>204</v>
       </c>
@@ -10930,7 +10942,7 @@
       <c r="BZ109" s="10"/>
       <c r="CA109" s="10"/>
     </row>
-    <row r="110" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>205</v>
       </c>
@@ -11021,7 +11033,7 @@
       <c r="BZ110" s="10"/>
       <c r="CA110" s="10"/>
     </row>
-    <row r="111" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>206</v>
       </c>
@@ -11112,7 +11124,7 @@
       <c r="BZ111" s="10"/>
       <c r="CA111" s="10"/>
     </row>
-    <row r="112" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>207</v>
       </c>
@@ -11203,7 +11215,7 @@
       <c r="BZ112" s="10"/>
       <c r="CA112" s="10"/>
     </row>
-    <row r="113" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>208</v>
       </c>
@@ -11294,7 +11306,7 @@
       <c r="BZ113" s="10"/>
       <c r="CA113" s="10"/>
     </row>
-    <row r="114" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>209</v>
       </c>
@@ -11385,7 +11397,7 @@
       <c r="BZ114" s="10"/>
       <c r="CA114" s="10"/>
     </row>
-    <row r="115" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>210</v>
       </c>
@@ -11476,7 +11488,7 @@
       <c r="BZ115" s="10"/>
       <c r="CA115" s="10"/>
     </row>
-    <row r="116" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>215</v>
       </c>
@@ -11561,7 +11573,7 @@
       <c r="BZ116" s="10"/>
       <c r="CA116" s="10"/>
     </row>
-    <row r="117" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>218</v>
       </c>
@@ -11646,7 +11658,7 @@
       <c r="BZ117" s="10"/>
       <c r="CA117" s="10"/>
     </row>
-    <row r="118" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>221</v>
       </c>
@@ -11741,7 +11753,7 @@
       <c r="BZ118" s="10"/>
       <c r="CA118" s="10"/>
     </row>
-    <row r="119" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>222</v>
       </c>
@@ -11836,7 +11848,7 @@
       <c r="BZ119" s="10"/>
       <c r="CA119" s="10"/>
     </row>
-    <row r="120" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>223</v>
       </c>
@@ -11931,7 +11943,7 @@
       <c r="BZ120" s="10"/>
       <c r="CA120" s="10"/>
     </row>
-    <row r="121" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>224</v>
       </c>
@@ -12026,7 +12038,7 @@
       <c r="BZ121" s="10"/>
       <c r="CA121" s="10"/>
     </row>
-    <row r="122" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>225</v>
       </c>
@@ -12121,7 +12133,7 @@
       <c r="BZ122" s="10"/>
       <c r="CA122" s="10"/>
     </row>
-    <row r="123" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>226</v>
       </c>
@@ -12206,7 +12218,7 @@
       <c r="BZ123" s="10"/>
       <c r="CA123" s="10"/>
     </row>
-    <row r="124" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>227</v>
       </c>
@@ -12303,7 +12315,7 @@
       <c r="BZ124" s="10"/>
       <c r="CA124" s="10"/>
     </row>
-    <row r="125" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>229</v>
       </c>
@@ -12388,7 +12400,7 @@
       <c r="BZ125" s="10"/>
       <c r="CA125" s="10"/>
     </row>
-    <row r="126" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>232</v>
       </c>
@@ -12473,7 +12485,7 @@
       <c r="BZ126" s="10"/>
       <c r="CA126" s="10"/>
     </row>
-    <row r="127" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:79" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>241</v>
       </c>
@@ -12499,11 +12511,10 @@
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
       <c r="W127" s="1"/>
-      <c r="X127" s="1" t="s">
+      <c r="Y127" s="1"/>
+      <c r="Z127" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="Y127" s="1"/>
-      <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
       <c r="AB127" s="1"/>
       <c r="AC127" s="1"/>
@@ -12558,7 +12569,7 @@
       <c r="BZ127" s="10"/>
       <c r="CA127" s="10"/>
     </row>
-    <row r="128" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="8"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -12639,7 +12650,7 @@
       <c r="BZ128" s="9"/>
       <c r="CA128" s="9"/>
     </row>
-    <row r="129" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="8"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -12720,7 +12731,7 @@
       <c r="BZ129" s="9"/>
       <c r="CA129" s="9"/>
     </row>
-    <row r="130" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -12801,7 +12812,7 @@
       <c r="BZ130" s="9"/>
       <c r="CA130" s="9"/>
     </row>
-    <row r="131" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="8"/>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
@@ -12882,7 +12893,7 @@
       <c r="BZ131" s="9"/>
       <c r="CA131" s="9"/>
     </row>
-    <row r="132" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
@@ -12963,7 +12974,7 @@
       <c r="BZ132" s="9"/>
       <c r="CA132" s="9"/>
     </row>
-    <row r="133" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="8"/>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
@@ -13044,7 +13055,7 @@
       <c r="BZ133" s="9"/>
       <c r="CA133" s="9"/>
     </row>
-    <row r="134" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="8"/>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
@@ -13125,7 +13136,7 @@
       <c r="BZ134" s="9"/>
       <c r="CA134" s="9"/>
     </row>
-    <row r="135" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="8"/>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
@@ -13206,7 +13217,7 @@
       <c r="BZ135" s="9"/>
       <c r="CA135" s="9"/>
     </row>
-    <row r="136" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
@@ -13287,7 +13298,7 @@
       <c r="BZ136" s="9"/>
       <c r="CA136" s="9"/>
     </row>
-    <row r="137" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
@@ -13368,7 +13379,7 @@
       <c r="BZ137" s="9"/>
       <c r="CA137" s="9"/>
     </row>
-    <row r="138" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
@@ -13449,7 +13460,7 @@
       <c r="BZ138" s="9"/>
       <c r="CA138" s="9"/>
     </row>
-    <row r="139" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
@@ -13530,7 +13541,7 @@
       <c r="BZ139" s="9"/>
       <c r="CA139" s="9"/>
     </row>
-    <row r="140" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="8"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
@@ -13611,7 +13622,7 @@
       <c r="BZ140" s="9"/>
       <c r="CA140" s="9"/>
     </row>
-    <row r="141" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="8"/>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
@@ -13692,7 +13703,7 @@
       <c r="BZ141" s="9"/>
       <c r="CA141" s="9"/>
     </row>
-    <row r="142" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
@@ -13773,7 +13784,7 @@
       <c r="BZ142" s="9"/>
       <c r="CA142" s="9"/>
     </row>
-    <row r="143" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="8"/>
       <c r="B143" s="8"/>
       <c r="C143" s="8"/>
@@ -13854,7 +13865,7 @@
       <c r="BZ143" s="9"/>
       <c r="CA143" s="9"/>
     </row>
-    <row r="144" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="8"/>
       <c r="B144" s="8"/>
       <c r="C144" s="8"/>
@@ -13935,7 +13946,7 @@
       <c r="BZ144" s="9"/>
       <c r="CA144" s="9"/>
     </row>
-    <row r="145" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="8"/>
       <c r="B145" s="8"/>
       <c r="C145" s="8"/>
@@ -14016,7 +14027,7 @@
       <c r="BZ145" s="9"/>
       <c r="CA145" s="9"/>
     </row>
-    <row r="146" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
@@ -14097,7 +14108,7 @@
       <c r="BZ146" s="9"/>
       <c r="CA146" s="9"/>
     </row>
-    <row r="147" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="8"/>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
@@ -14178,7 +14189,7 @@
       <c r="BZ147" s="9"/>
       <c r="CA147" s="9"/>
     </row>
-    <row r="148" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
@@ -14259,7 +14270,7 @@
       <c r="BZ148" s="9"/>
       <c r="CA148" s="9"/>
     </row>
-    <row r="149" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="8"/>
       <c r="B149" s="8"/>
       <c r="C149" s="8"/>
@@ -14340,7 +14351,7 @@
       <c r="BZ149" s="9"/>
       <c r="CA149" s="9"/>
     </row>
-    <row r="150" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="8"/>
@@ -14421,7 +14432,7 @@
       <c r="BZ150" s="9"/>
       <c r="CA150" s="9"/>
     </row>
-    <row r="151" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="8"/>
       <c r="B151" s="8"/>
       <c r="C151" s="8"/>
@@ -14502,7 +14513,7 @@
       <c r="BZ151" s="9"/>
       <c r="CA151" s="9"/>
     </row>
-    <row r="152" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="8"/>
@@ -14583,7 +14594,7 @@
       <c r="BZ152" s="9"/>
       <c r="CA152" s="9"/>
     </row>
-    <row r="153" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="8"/>
       <c r="B153" s="8"/>
       <c r="C153" s="8"/>
@@ -14664,7 +14675,7 @@
       <c r="BZ153" s="9"/>
       <c r="CA153" s="9"/>
     </row>
-    <row r="154" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="8"/>
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
@@ -14745,7 +14756,7 @@
       <c r="BZ154" s="9"/>
       <c r="CA154" s="9"/>
     </row>
-    <row r="155" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="8"/>
       <c r="B155" s="8"/>
       <c r="C155" s="8"/>
@@ -14826,7 +14837,7 @@
       <c r="BZ155" s="9"/>
       <c r="CA155" s="9"/>
     </row>
-    <row r="156" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="8"/>
       <c r="B156" s="8"/>
       <c r="C156" s="8"/>
@@ -14907,7 +14918,7 @@
       <c r="BZ156" s="9"/>
       <c r="CA156" s="9"/>
     </row>
-    <row r="157" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="8"/>
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
@@ -14988,7 +14999,7 @@
       <c r="BZ157" s="9"/>
       <c r="CA157" s="9"/>
     </row>
-    <row r="158" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="8"/>
       <c r="B158" s="8"/>
       <c r="C158" s="8"/>
@@ -15069,7 +15080,7 @@
       <c r="BZ158" s="9"/>
       <c r="CA158" s="9"/>
     </row>
-    <row r="159" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
@@ -15150,7 +15161,7 @@
       <c r="BZ159" s="9"/>
       <c r="CA159" s="9"/>
     </row>
-    <row r="160" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="8"/>
       <c r="B160" s="8"/>
       <c r="C160" s="8"/>
@@ -15231,7 +15242,7 @@
       <c r="BZ160" s="9"/>
       <c r="CA160" s="9"/>
     </row>
-    <row r="161" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="8"/>
       <c r="B161" s="8"/>
       <c r="C161" s="8"/>
@@ -15312,7 +15323,7 @@
       <c r="BZ161" s="9"/>
       <c r="CA161" s="9"/>
     </row>
-    <row r="162" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
       <c r="B162" s="8"/>
       <c r="C162" s="8"/>
@@ -15393,7 +15404,7 @@
       <c r="BZ162" s="9"/>
       <c r="CA162" s="9"/>
     </row>
-    <row r="163" spans="1:79" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:79" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="8"/>
       <c r="B163" s="8"/>
       <c r="C163" s="8"/>
@@ -15474,7 +15485,7 @@
       <c r="BZ163" s="9"/>
       <c r="CA163" s="9"/>
     </row>
-    <row r="164" spans="1:79" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>

</xml_diff>

<commit_message>
Errores de analizadores corregidos
</commit_message>
<xml_diff>
--- a/TablaSintactica.xlsx
+++ b/TablaSintactica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\OneDrive\Documentos\University\Archivos\PDF's\Autómatas\Programas\Compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2E49C-89ED-4ED1-A9BB-4FC8C01D7A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E72A64-A9F9-473C-8341-7A0DD0B7ACDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{D62EC496-1556-4E0C-9A3E-7AF50D9FA4F9}"/>
   </bookViews>
@@ -1208,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E59CA23-57F3-4C77-80B4-8B27E4C8042E}">
   <dimension ref="A1:CY164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>